<commit_message>
completed MML4 mapping updates
</commit_message>
<xml_diff>
--- a/mapping/mml4_progress_course_mapping.xlsx
+++ b/mapping/mml4_progress_course_mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="357">
   <si>
     <t>Archetype</t>
     <phoneticPr fontId="1"/>
@@ -190,15 +190,9 @@
     <t>1.2.1.3.3.1.</t>
   </si>
   <si>
-    <t>1.2.1.3.4.</t>
-  </si>
-  <si>
     <t>mmlPc:rxRecord</t>
   </si>
   <si>
-    <t>1.2.1.3.4.1.</t>
-  </si>
-  <si>
     <t>1.2.1.3.5.</t>
   </si>
   <si>
@@ -239,9 +233,6 @@
   </si>
   <si>
     <t>mmlPc:rxOrder</t>
-  </si>
-  <si>
-    <t>1.2.1.5.2.1.</t>
   </si>
   <si>
     <t>1.2.1.5.3.</t>
@@ -597,12 +588,708 @@
     <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0001]/items[openEHR-EHR-OBSERVATION.story.v1 and name/value='Story/History']/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.symptom.v1 and name/value='Symptom']/items[at0033]/items[at0060]/value</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>mmlPs:PrescriptionModule</t>
+  </si>
+  <si>
+    <t>mmlPs:issuedTo</t>
+  </si>
+  <si>
+    <t>issued to</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_TEXT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:medication</t>
+  </si>
+  <si>
+    <t>mmlPs:medicine</t>
+  </si>
+  <si>
+    <t>mmlPs:name</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:code</t>
+  </si>
+  <si>
+    <t>mmlPs:system</t>
+  </si>
+  <si>
+    <t>#REQUIRED</t>
+  </si>
+  <si>
+    <t>値は常に"="</t>
+    <rPh sb="0" eb="1">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ツネ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:dose</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>Amount</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_QUANTITY</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:doseUnit</t>
+  </si>
+  <si>
+    <t>mmPs:frequencyPerDay</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmPs:startDate</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Start date/time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_DATE_TIME</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmPs:duration</t>
+  </si>
+  <si>
+    <t>Direction duration</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_DURATION</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:instruction</t>
+  </si>
+  <si>
+    <t>Patient instruction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:PRN</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>As requied</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DV_BOOLEAN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:route</t>
+  </si>
+  <si>
+    <t>Route</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:form</t>
+  </si>
+  <si>
+    <t>Preparation form</t>
+  </si>
+  <si>
+    <t>mmlPs:batchNo</t>
+  </si>
+  <si>
+    <t>Direction sequence</t>
+  </si>
+  <si>
+    <t>DV_COUNT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:brandSubstitutionPermitted</t>
+  </si>
+  <si>
+    <t>substitution permitted</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:longTerm</t>
+  </si>
+  <si>
+    <t>long term</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:additionalInstruction</t>
+  </si>
+  <si>
+    <t>Additional instruction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlPs:narcoticPrescriptionLicenseNumber</t>
+  </si>
+  <si>
+    <t>narcotic prescription license number</t>
+  </si>
+  <si>
+    <t>mmlInj:InjectionModule</t>
+  </si>
+  <si>
+    <t>mmlInj:medication</t>
+  </si>
+  <si>
+    <t>mmlInj:medicine</t>
+  </si>
+  <si>
+    <t>mmlInj:name</t>
+  </si>
+  <si>
+    <t>Medication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlInj:code</t>
+  </si>
+  <si>
+    <t>mmlInj:system</t>
+  </si>
+  <si>
+    <t>mmlInj:dose</t>
+  </si>
+  <si>
+    <t>mmlInj:doseUnit</t>
+  </si>
+  <si>
+    <t>mmInj:startDateTime</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>Order start date/time</t>
+  </si>
+  <si>
+    <t>mmInj:endDateTime</t>
+  </si>
+  <si>
+    <t>Order stop date/time</t>
+  </si>
+  <si>
+    <t>mmlInj:instruction</t>
+  </si>
+  <si>
+    <t>Administration instruction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlInj:route</t>
+  </si>
+  <si>
+    <t>mmlInj:site</t>
+  </si>
+  <si>
+    <t>Site</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlInj:deliveryMethod</t>
+  </si>
+  <si>
+    <t>Delivery method</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlInj:batchNo</t>
+  </si>
+  <si>
+    <t>mmlInj:additionalInstruction</t>
+  </si>
+  <si>
+    <t>mmlInj:narcoticPrescriptionLicenseNumber</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.1.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.1.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.11</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.12</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.13</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.2.14</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.1.3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.2.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.2.1.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4.2.1.1.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.1.1</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.1.2</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.2</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.3</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.4</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.5</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.6</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.7</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.8</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.9</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.10</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.1.11</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4..2.1.2</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0070]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0070]/mappings/target/code_string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0070]/mappings/target/terminology_id/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0070]/mappings/match</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[at0144]/magnitude</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[at0144]/units</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[openEHR-EHR-CLUSTER.daily_timing.v0]/items[at0003]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0113]/items[at0012]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0066]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0105]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[openEHR-EHR-CLUSTER.daily_timing.v0]/items[at0024]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0091]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[openEHR-EHR-CLUSTER.medication_preparation.v0]/items[at0071]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0057]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0129]/items[at0132]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0044]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0070]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0070]/mappings/target/code_string</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0070]/mappings/target/terminology_id/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0070]/mappings/match</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[at0144]/magnitude</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[at0144]/units</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0113]/items[at0012]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0113]/items[at0013]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0133]/items[at0108]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0091]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0133]/items[at0092]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0133]/items[at0094]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0056]/items[at0057]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0044]/value</t>
+  </si>
+  <si>
+    <t>1.2.1.3.4.3.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.1.2</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.2</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.3</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.4</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.5</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.6</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.7</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.8</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.9</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.10</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.11</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.12</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.13</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.14</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.3</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.2.1</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.2.1.1</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2.2.1.1.1</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.1.1</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.1.2</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.2</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.3</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.4</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.5</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.6</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.7</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.8</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.9</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.10</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.1.11</t>
+  </si>
+  <si>
+    <t>1.2.1.5.2..2.1.2</t>
+  </si>
+  <si>
+    <t>1.2.1.5.3.1.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.2.1.5.2.1.2.1.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0070]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0070]/mappings/target/code_string</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0070]/mappings/target/terminology_id/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0070]/mappings/match</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[at0144]/magnitude</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[at0144]/units</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[openEHR-EHR-CLUSTER.daily_timing.v0]/items[at0003]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0113]/items[at0012]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0066]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0105]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[openEHR-EHR-CLUSTER.daily_timing.v0]/items[at0024]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0091]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[openEHR-EHR-CLUSTER.medication_preparation.v0]/items[at0071]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0056]/items[at0057]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0129]/items[at0132]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Prescription']/activities[at0001]/description[at0002]/items[at0044]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0070]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0070]/mappings/target/code_string</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0070]/mappings/target/terminology_id/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0070]/mappings/match</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[at0144]/magnitude</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0056]/items[at0058]/items[at0144]/units</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0113]/items[at0012]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0113]/items[at0013]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0133]/items[at0108]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0091]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0133]/items[at0092]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0133]/items[at0094]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0056]/items[at0057]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-INSTRUCTION.medication_order.v0 and name/value='Injection']/activities[at0001]/description[at0002]/items[at0044]/value</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,8 +1313,17 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,6 +1333,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,7 +1372,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -691,6 +1393,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -993,16 +1725,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="25.875" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="28.75" customWidth="1"/>
     <col min="3" max="3" width="11.625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
@@ -1018,7 +1750,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2"/>
       <c r="H2" t="s">
@@ -1028,7 +1760,7 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
@@ -1064,7 +1796,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -1081,16 +1813,16 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -1133,7 +1865,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="H8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -1152,13 +1884,13 @@
       </c>
       <c r="F9" s="3"/>
       <c r="I9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -1175,13 +1907,13 @@
       </c>
       <c r="F10" s="3"/>
       <c r="I10" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -1198,7 +1930,7 @@
       </c>
       <c r="F11" s="3"/>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -1215,16 +1947,16 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="H12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
@@ -1241,7 +1973,7 @@
       </c>
       <c r="F13" s="3"/>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
@@ -1258,13 +1990,13 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="I14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
@@ -1283,13 +2015,13 @@
       </c>
       <c r="F15" s="3"/>
       <c r="I15" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
@@ -1300,16 +2032,16 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="H16" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
@@ -1342,16 +2074,16 @@
       </c>
       <c r="F18" s="3"/>
       <c r="H18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
@@ -1368,7 +2100,7 @@
       </c>
       <c r="F19" s="3"/>
       <c r="H19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
@@ -1385,7 +2117,7 @@
       </c>
       <c r="F20" s="3"/>
       <c r="H20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
@@ -1402,13 +2134,13 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
@@ -1425,13 +2157,13 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="I22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
@@ -1450,16 +2182,16 @@
       </c>
       <c r="F23" s="3"/>
       <c r="H23" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="J23" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
@@ -1490,16 +2222,16 @@
       </c>
       <c r="F25" s="3"/>
       <c r="H25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
@@ -1518,16 +2250,16 @@
       </c>
       <c r="F26" s="3"/>
       <c r="H26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
@@ -1544,24 +2276,24 @@
       </c>
       <c r="F27" s="3"/>
       <c r="H27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
@@ -1572,417 +2304,2115 @@
       </c>
       <c r="F28" s="3"/>
       <c r="H28" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A29" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A30" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="K31" s="9"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A32" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A33" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="I33" t="s">
+        <v>158</v>
+      </c>
+      <c r="J33" t="s">
+        <v>154</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A34" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="K34" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="K35" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="J36" t="s">
+        <v>162</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A37" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="I37" t="s">
+        <v>165</v>
+      </c>
+      <c r="J37" t="s">
+        <v>166</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A38" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="K38" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A39" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="I39" t="s">
+        <v>169</v>
+      </c>
+      <c r="J39" t="s">
+        <v>166</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A40" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="I40" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" t="s">
+        <v>173</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A41" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="I41" t="s">
+        <v>175</v>
+      </c>
+      <c r="J41" t="s">
+        <v>176</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A42" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="I42" t="s">
+        <v>178</v>
+      </c>
+      <c r="J42" t="s">
+        <v>154</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A43" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="I43" t="s">
+        <v>181</v>
+      </c>
+      <c r="J43" t="s">
+        <v>182</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A44" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="I44" t="s">
+        <v>184</v>
+      </c>
+      <c r="J44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A45" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="I45" t="s">
+        <v>186</v>
+      </c>
+      <c r="J45" t="s">
+        <v>154</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A46" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="I46" t="s">
+        <v>188</v>
+      </c>
+      <c r="J46" t="s">
+        <v>189</v>
+      </c>
+      <c r="K46" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A47" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="I47" t="s">
+        <v>191</v>
+      </c>
+      <c r="J47" t="s">
+        <v>182</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A48" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K48" s="12"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A49" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="I49" t="s">
+        <v>195</v>
+      </c>
+      <c r="J49" t="s">
+        <v>154</v>
+      </c>
+      <c r="K49" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A50" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="J50" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="K50" s="12"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A51" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A52" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A53" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A54" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="I54" t="s">
+        <v>202</v>
+      </c>
+      <c r="J54" t="s">
+        <v>154</v>
+      </c>
+      <c r="K54" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A55" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="8"/>
+      <c r="K55" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A56" s="15"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="K56" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A57" s="15"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="J57" t="s">
+        <v>162</v>
+      </c>
+      <c r="K57" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A58" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="I58" t="s">
+        <v>165</v>
+      </c>
+      <c r="J58" t="s">
+        <v>166</v>
+      </c>
+      <c r="K58" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A59" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="K59" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A60" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="8"/>
+      <c r="I60" t="s">
+        <v>209</v>
+      </c>
+      <c r="J60" t="s">
+        <v>173</v>
+      </c>
+      <c r="K60" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A61" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="I61" t="s">
+        <v>211</v>
+      </c>
+      <c r="J61" t="s">
+        <v>173</v>
+      </c>
+      <c r="K61" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A62" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="8"/>
+      <c r="I62" t="s">
+        <v>213</v>
+      </c>
+      <c r="J62" t="s">
+        <v>154</v>
+      </c>
+      <c r="K62" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A63" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="8"/>
+      <c r="I63" t="s">
+        <v>184</v>
+      </c>
+      <c r="J63" t="s">
+        <v>154</v>
+      </c>
+      <c r="K63" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A64" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="8"/>
+      <c r="I64" t="s">
+        <v>216</v>
+      </c>
+      <c r="J64" t="s">
+        <v>154</v>
+      </c>
+      <c r="K64" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A65" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="8"/>
+      <c r="I65" t="s">
+        <v>218</v>
+      </c>
+      <c r="J65" t="s">
+        <v>154</v>
+      </c>
+      <c r="K65" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A66" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="8"/>
+      <c r="I66" t="s">
+        <v>188</v>
+      </c>
+      <c r="J66" t="s">
+        <v>189</v>
+      </c>
+      <c r="K66" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A67" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="8"/>
+      <c r="I67" t="s">
+        <v>195</v>
+      </c>
+      <c r="J67" t="s">
+        <v>154</v>
+      </c>
+      <c r="K67" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A68" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="11"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="J68" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K68" s="12"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A69" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="H69" t="s">
         <v>99</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I69" t="s">
+        <v>100</v>
+      </c>
+      <c r="J69" t="s">
+        <v>130</v>
+      </c>
+      <c r="K69" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A70" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="H70" t="s">
+        <v>96</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K70" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A71" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="H71" t="s">
+        <v>99</v>
+      </c>
+      <c r="I71" t="s">
+        <v>100</v>
+      </c>
+      <c r="J71" t="s">
+        <v>130</v>
+      </c>
+      <c r="K71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A72" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="3"/>
+      <c r="H72" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A73" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="3"/>
+      <c r="I73" t="s">
+        <v>77</v>
+      </c>
+      <c r="J73" t="s">
+        <v>113</v>
+      </c>
+      <c r="K73" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A74" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A75" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="3"/>
+      <c r="H75" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I75" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="J75" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K75" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="K76" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A77" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="H29" t="s">
+      <c r="F77" s="3"/>
+      <c r="H77" t="s">
+        <v>99</v>
+      </c>
+      <c r="I77" t="s">
+        <v>100</v>
+      </c>
+      <c r="J77" t="s">
+        <v>129</v>
+      </c>
+      <c r="K77" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A78" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="3"/>
+      <c r="H78" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K78" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K79" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A80" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="K80" s="9"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A81" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="11"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="J81" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K81" s="12"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A82" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="8"/>
+      <c r="K82" s="9"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A83" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="K83" s="9"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A84" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="I84" t="s">
+        <v>158</v>
+      </c>
+      <c r="J84" t="s">
+        <v>154</v>
+      </c>
+      <c r="K84" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A85" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="8"/>
+      <c r="K85" s="9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A86" s="7"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F86" s="8"/>
+      <c r="K86" s="9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A87" s="7"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+      <c r="J87" t="s">
+        <v>162</v>
+      </c>
+      <c r="K87" s="9" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A88" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="I88" t="s">
+        <v>165</v>
+      </c>
+      <c r="J88" t="s">
+        <v>166</v>
+      </c>
+      <c r="K88" s="9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A89" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="K89" s="9" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A90" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+      <c r="I90" t="s">
+        <v>169</v>
+      </c>
+      <c r="J90" t="s">
+        <v>166</v>
+      </c>
+      <c r="K90" s="9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A91" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="8"/>
+      <c r="I91" t="s">
+        <v>172</v>
+      </c>
+      <c r="J91" t="s">
+        <v>173</v>
+      </c>
+      <c r="K91" s="9" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A92" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="I92" t="s">
+        <v>175</v>
+      </c>
+      <c r="J92" t="s">
+        <v>176</v>
+      </c>
+      <c r="K92" s="9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A93" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" s="8"/>
+      <c r="I93" t="s">
+        <v>178</v>
+      </c>
+      <c r="J93" t="s">
+        <v>154</v>
+      </c>
+      <c r="K93" s="9" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A94" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="8"/>
+      <c r="I94" t="s">
+        <v>181</v>
+      </c>
+      <c r="J94" t="s">
+        <v>182</v>
+      </c>
+      <c r="K94" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A95" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="8"/>
+      <c r="I95" t="s">
+        <v>184</v>
+      </c>
+      <c r="J95" t="s">
+        <v>154</v>
+      </c>
+      <c r="K95" s="9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A96" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="8"/>
+      <c r="I96" t="s">
+        <v>186</v>
+      </c>
+      <c r="J96" t="s">
+        <v>154</v>
+      </c>
+      <c r="K96" s="9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A97" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="8"/>
+      <c r="I97" t="s">
+        <v>188</v>
+      </c>
+      <c r="J97" t="s">
+        <v>189</v>
+      </c>
+      <c r="K97" s="9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A98" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" s="8"/>
+      <c r="I98" t="s">
+        <v>191</v>
+      </c>
+      <c r="J98" t="s">
+        <v>182</v>
+      </c>
+      <c r="K98" s="9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A99" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E99" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" s="11"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="J99" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K99" s="12"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A100" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="8"/>
+      <c r="I100" t="s">
+        <v>195</v>
+      </c>
+      <c r="J100" t="s">
+        <v>154</v>
+      </c>
+      <c r="K100" s="9" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A101" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B101" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101" s="12"/>
+      <c r="D101" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101" s="11"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="J101" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="K101" s="12"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A102" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A103" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F103" s="8"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A104" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A105" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8"/>
+      <c r="I105" t="s">
+        <v>202</v>
+      </c>
+      <c r="J105" t="s">
+        <v>154</v>
+      </c>
+      <c r="K105" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A106" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="8"/>
+      <c r="K106" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A107" s="15"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+      <c r="K107" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A108" s="15"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+      <c r="J108" t="s">
+        <v>162</v>
+      </c>
+      <c r="K108" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A109" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8"/>
+      <c r="I109" t="s">
+        <v>165</v>
+      </c>
+      <c r="J109" t="s">
+        <v>166</v>
+      </c>
+      <c r="K109" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A110" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+      <c r="K110" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A111" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E111" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" s="8"/>
+      <c r="I111" t="s">
+        <v>209</v>
+      </c>
+      <c r="J111" t="s">
+        <v>173</v>
+      </c>
+      <c r="K111" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A112" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" s="8"/>
+      <c r="I112" t="s">
+        <v>211</v>
+      </c>
+      <c r="J112" t="s">
+        <v>173</v>
+      </c>
+      <c r="K112" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A113" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F113" s="8"/>
+      <c r="I113" t="s">
+        <v>213</v>
+      </c>
+      <c r="J113" t="s">
+        <v>154</v>
+      </c>
+      <c r="K113" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A114" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F114" s="8"/>
+      <c r="I114" t="s">
+        <v>184</v>
+      </c>
+      <c r="J114" t="s">
+        <v>154</v>
+      </c>
+      <c r="K114" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A115" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" s="8"/>
+      <c r="I115" t="s">
+        <v>216</v>
+      </c>
+      <c r="J115" t="s">
+        <v>154</v>
+      </c>
+      <c r="K115" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A116" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E116" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F116" s="8"/>
+      <c r="I116" t="s">
+        <v>218</v>
+      </c>
+      <c r="J116" t="s">
+        <v>154</v>
+      </c>
+      <c r="K116" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A117" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E117" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F117" s="8"/>
+      <c r="I117" t="s">
+        <v>188</v>
+      </c>
+      <c r="J117" t="s">
+        <v>189</v>
+      </c>
+      <c r="K117" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A118" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F118" s="8"/>
+      <c r="I118" t="s">
+        <v>195</v>
+      </c>
+      <c r="J118" t="s">
+        <v>154</v>
+      </c>
+      <c r="K118" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="27" x14ac:dyDescent="0.15">
+      <c r="A119" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="B119" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C119" s="11"/>
+      <c r="D119" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F119" s="11"/>
+      <c r="G119" s="12"/>
+      <c r="H119" s="12"/>
+      <c r="I119" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="J119" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K119" s="12"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A120" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F120" s="3"/>
+      <c r="H120" t="s">
+        <v>99</v>
+      </c>
+      <c r="I120" t="s">
+        <v>100</v>
+      </c>
+      <c r="J120" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="K120" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A121" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F121" s="3"/>
+      <c r="H121" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I121" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J121" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K121" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A122" s="3"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="H122" s="5"/>
+      <c r="I122" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J122" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K122" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A123" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F123" s="3"/>
+      <c r="H123" t="s">
+        <v>99</v>
+      </c>
+      <c r="I123" t="s">
+        <v>100</v>
+      </c>
+      <c r="J123" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="K123" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A124" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" s="3"/>
+      <c r="H124" t="s">
+        <v>94</v>
+      </c>
+      <c r="I124" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J124" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K124" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B126" s="4"/>
+    </row>
+    <row r="127" spans="1:11" ht="54" x14ac:dyDescent="0.15">
+      <c r="B127" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I29" t="s">
-        <v>103</v>
-      </c>
-      <c r="J29" t="s">
-        <v>133</v>
-      </c>
-      <c r="K29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A30" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="H30" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="3"/>
-      <c r="H31" t="s">
-        <v>102</v>
-      </c>
-      <c r="I31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J31" t="s">
-        <v>133</v>
-      </c>
-      <c r="K31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="H32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="I33" t="s">
-        <v>80</v>
-      </c>
-      <c r="J33" t="s">
-        <v>116</v>
-      </c>
-      <c r="K33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A34" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A35" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="3"/>
-      <c r="H35" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I35" s="4" t="s">
+      <c r="I127" t="s">
         <v>104</v>
       </c>
-      <c r="J35" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="K35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="6" t="s">
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I128" t="s">
         <v>106</v>
       </c>
-      <c r="J36" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K36" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A37" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="3"/>
-      <c r="H37" t="s">
-        <v>102</v>
-      </c>
-      <c r="I37" t="s">
-        <v>103</v>
-      </c>
-      <c r="J37" t="s">
-        <v>132</v>
-      </c>
-      <c r="K37" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A38" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="H38" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K38" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K39" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A40" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="H40" t="s">
-        <v>102</v>
-      </c>
-      <c r="I40" t="s">
-        <v>103</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="K40" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A41" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="3"/>
-      <c r="H41" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K41" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K42" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A43" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" s="3"/>
-      <c r="H43" t="s">
-        <v>102</v>
-      </c>
-      <c r="I43" t="s">
-        <v>103</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="K43" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A44" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="H44" t="s">
-        <v>97</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K44" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B46" s="4"/>
-    </row>
-    <row r="47" spans="1:11" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="B47" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="I47" t="s">
+    </row>
+    <row r="129" spans="9:9" x14ac:dyDescent="0.15">
+      <c r="I129" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="I48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.15">
-      <c r="I49" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed phisical examination ext ref
</commit_message>
<xml_diff>
--- a/mapping/mml4_progress_course_mapping.xlsx
+++ b/mapping/mml4_progress_course_mapping.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$158</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="396">
   <si>
     <t>Attribute</t>
   </si>
@@ -1139,10 +1139,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>URI to original data1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>URI to original data2</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1385,6 +1381,18 @@
   </si>
   <si>
     <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='TxOrder']/protocol[at0008]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1]/protocol[at0007]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1]/protocol[at0007]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0004]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1]/protocol[at0007]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0003]/value</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1681,51 +1689,7 @@
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -2046,10 +2010,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K153"/>
+  <dimension ref="A1:K158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K148" sqref="K148"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2237,7 +2201,7 @@
         <v>184</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -2314,13 +2278,13 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="I14" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>184</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
@@ -2548,66 +2512,59 @@
       <c r="H25" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>220</v>
-      </c>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="H26" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>184</v>
+      <c r="A26" s="4"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="41" t="s">
+        <v>362</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26"/>
+      <c r="I26" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="J26" t="s">
+        <v>363</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>333</v>
+        <v>393</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="H27" s="1" t="s">
-        <v>183</v>
+      <c r="A27" s="4"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="41" t="s">
+        <v>364</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27"/>
+      <c r="I27" s="43" t="s">
+        <v>371</v>
+      </c>
+      <c r="J27" t="s">
+        <v>365</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A28" s="14"/>
-      <c r="B28" s="40"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="41" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D28" s="41" t="s">
         <v>5</v>
@@ -2616,279 +2573,283 @@
       <c r="F28" s="42"/>
       <c r="G28" s="43"/>
       <c r="H28"/>
-      <c r="I28" s="44" t="s">
-        <v>371</v>
+      <c r="I28" s="43" t="s">
+        <v>372</v>
       </c>
       <c r="J28" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>374</v>
+        <v>395</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A29" s="14"/>
-      <c r="B29" s="40"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="41" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>5</v>
+        <v>368</v>
       </c>
       <c r="E29" s="42"/>
       <c r="F29" s="42"/>
       <c r="G29" s="43"/>
       <c r="H29"/>
-      <c r="I29" s="43" t="s">
+      <c r="I29" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A30" s="4"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="H31" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="H32" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A33" s="14"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="41" t="s">
+        <v>362</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="43"/>
+      <c r="H33"/>
+      <c r="I33" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="J33" t="s">
+        <v>363</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A34" s="14"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="41" t="s">
+        <v>364</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="43"/>
+      <c r="H34"/>
+      <c r="I34" s="43" t="s">
+        <v>371</v>
+      </c>
+      <c r="J34" t="s">
+        <v>365</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A35" s="14"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41" t="s">
+        <v>366</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="43"/>
+      <c r="H35"/>
+      <c r="I35" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="J29" t="s">
-        <v>366</v>
-      </c>
-      <c r="K29" s="1" t="s">
+      <c r="J35" t="s">
+        <v>365</v>
+      </c>
+      <c r="K35" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A30" s="14"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="41" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A36" s="14"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="41" t="s">
         <v>367</v>
       </c>
-      <c r="D30" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="H30"/>
-      <c r="I30" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="J30" t="s">
-        <v>366</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A31" s="14"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="41" t="s">
+      <c r="D36" s="41" t="s">
         <v>368</v>
       </c>
-      <c r="D31" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="43"/>
-      <c r="H31"/>
-      <c r="I31" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="J31" s="1" t="s">
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="43"/>
+      <c r="H36"/>
+      <c r="I36" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A32" s="14" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A37" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B37" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="14"/>
-      <c r="H32" s="1" t="s">
+      <c r="C37" s="14"/>
+      <c r="D37" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="14"/>
+      <c r="H37" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I37" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J37" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A33" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="K33" s="8"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A34" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="16"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="K34" s="9"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A35" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="16"/>
-      <c r="K35" s="8"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A36" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B36" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="K36" s="8"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A37" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="I37" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>264</v>
+      <c r="K37" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A38" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>81</v>
+        <v>138</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>75</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>9</v>
-      </c>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
       <c r="F38" s="16"/>
-      <c r="K38" s="8" t="s">
-        <v>272</v>
-      </c>
+      <c r="K38" s="8"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A39" s="15"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>5</v>
-      </c>
+      <c r="A39" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
       <c r="E39" s="16" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="F39" s="16"/>
-      <c r="K39" s="8" t="s">
-        <v>273</v>
-      </c>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K39" s="9"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A40" s="15"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>78</v>
+      </c>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
+      <c r="E40" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="F40" s="16"/>
-      <c r="J40" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>265</v>
-      </c>
+      <c r="K40" s="8"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A41" s="15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C41" s="16"/>
-      <c r="D41" s="16" t="s">
-        <v>86</v>
-      </c>
+      <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
-      <c r="I41" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>275</v>
-      </c>
+      <c r="K41" s="8"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A42" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B42" s="30" t="s">
-        <v>88</v>
+        <v>142</v>
+      </c>
+      <c r="B42" s="31" t="s">
+        <v>80</v>
       </c>
       <c r="C42" s="16"/>
       <c r="D42" s="16" t="s">
@@ -2896,189 +2857,160 @@
       </c>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
+      <c r="I42" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="K42" s="8" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B43" s="30" t="s">
-        <v>89</v>
+        <v>143</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>81</v>
       </c>
       <c r="C43" s="16"/>
       <c r="D43" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E43" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="F43" s="16"/>
-      <c r="I43" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="K43" s="8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A44" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="B44" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="16"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="D44" s="16" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="F44" s="16"/>
-      <c r="I44" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="K44" s="8" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A45" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" s="30" t="s">
-        <v>93</v>
-      </c>
+      <c r="A45" s="15"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="16"/>
-      <c r="D45" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>7</v>
-      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
       <c r="F45" s="16"/>
-      <c r="I45" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="J45" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A46" s="15" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C46" s="16"/>
       <c r="D46" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E46" s="16"/>
       <c r="F46" s="16"/>
       <c r="I46" s="6" t="s">
-        <v>97</v>
+        <v>311</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>212</v>
+        <v>87</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A47" s="15" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E47" s="16"/>
       <c r="F47" s="16"/>
-      <c r="I47" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="K47" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A48" s="15" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C48" s="16"/>
       <c r="D48" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E48" s="16"/>
       <c r="F48" s="16"/>
       <c r="I48" s="6" t="s">
-        <v>102</v>
+        <v>319</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A49" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B49" s="31" t="s">
-        <v>103</v>
+        <v>147</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="C49" s="16"/>
       <c r="D49" s="16" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="E49" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F49" s="16"/>
       <c r="I49" s="6" t="s">
-        <v>104</v>
+        <v>315</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A50" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" s="31" t="s">
-        <v>105</v>
+        <v>148</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="C50" s="16"/>
       <c r="D50" s="16" t="s">
@@ -3089,46 +3021,46 @@
       </c>
       <c r="F50" s="16"/>
       <c r="I50" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A51" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B51" s="31" t="s">
-        <v>108</v>
+        <v>149</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>96</v>
       </c>
       <c r="C51" s="16"/>
       <c r="D51" s="16" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F51" s="16"/>
       <c r="I51" s="6" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>100</v>
+        <v>212</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A52" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B52" s="31" t="s">
-        <v>110</v>
+        <v>150</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>98</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16" t="s">
@@ -3138,22 +3070,22 @@
         <v>7</v>
       </c>
       <c r="F52" s="16"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="J52" s="9" t="s">
+      <c r="I52" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K52" s="9"/>
+      <c r="K52" s="8" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A53" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B53" s="31" t="s">
-        <v>112</v>
+        <v>151</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16" t="s">
@@ -3164,21 +3096,21 @@
       </c>
       <c r="F53" s="16"/>
       <c r="I53" s="6" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A54" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>114</v>
+        <v>152</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16" t="s">
@@ -3188,154 +3120,185 @@
         <v>7</v>
       </c>
       <c r="F54" s="16"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="J54" s="11" t="s">
+      <c r="I54" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K54" s="9"/>
+      <c r="K54" s="8" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A55" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="B55" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
+      <c r="A55" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="16"/>
+      <c r="I55" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A56" s="19" t="s">
-        <v>347</v>
-      </c>
-      <c r="B56" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="17"/>
+      <c r="A56" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="16"/>
+      <c r="I56" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A57" s="19" t="s">
-        <v>349</v>
-      </c>
-      <c r="B57" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
+      <c r="A57" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="16"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K57" s="9"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A58" s="19" t="s">
-        <v>350</v>
-      </c>
-      <c r="B58" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
+      <c r="A58" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="16"/>
       <c r="I58" s="6" t="s">
-        <v>310</v>
+        <v>113</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K58" s="1" t="s">
-        <v>226</v>
+      <c r="K58" s="8" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A59" s="19" t="s">
-        <v>351</v>
-      </c>
-      <c r="B59" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="17"/>
-      <c r="K59" s="1" t="s">
-        <v>227</v>
-      </c>
+      <c r="A59" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="16"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J59" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K59" s="9"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A60" s="19"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>5</v>
-      </c>
+      <c r="A60" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="B60" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
-      <c r="K60" s="1" t="s">
-        <v>228</v>
-      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A61" s="19"/>
-      <c r="B61" s="17"/>
+      <c r="A61" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="B61" s="33" t="s">
+        <v>117</v>
+      </c>
       <c r="C61" s="17"/>
       <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
+      <c r="E61" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="F61" s="17"/>
-      <c r="J61" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A62" s="19" t="s">
-        <v>352</v>
-      </c>
-      <c r="B62" s="36" t="s">
-        <v>122</v>
+        <v>348</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>118</v>
       </c>
       <c r="C62" s="17"/>
-      <c r="D62" s="17" t="s">
-        <v>86</v>
-      </c>
+      <c r="D62" s="17"/>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
-      <c r="I62" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A63" s="19" t="s">
-        <v>353</v>
-      </c>
-      <c r="B63" s="36" t="s">
-        <v>123</v>
+        <v>349</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>119</v>
       </c>
       <c r="C63" s="17"/>
       <c r="D63" s="17" t="s">
@@ -3343,191 +3306,160 @@
       </c>
       <c r="E63" s="17"/>
       <c r="F63" s="17"/>
+      <c r="I63" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="K63" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A64" s="19" t="s">
-        <v>354</v>
-      </c>
-      <c r="B64" s="36" t="s">
-        <v>124</v>
+        <v>350</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>120</v>
       </c>
       <c r="C64" s="17"/>
       <c r="D64" s="17" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F64" s="17"/>
-      <c r="I64" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="K64" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A65" s="19" t="s">
-        <v>355</v>
-      </c>
-      <c r="B65" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="17"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="17" t="s">
+        <v>121</v>
+      </c>
       <c r="D65" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="E65" s="17" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E65" s="17"/>
       <c r="F65" s="17"/>
-      <c r="I65" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J65" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="K65" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A66" s="19" t="s">
-        <v>356</v>
-      </c>
-      <c r="B66" s="36" t="s">
-        <v>128</v>
-      </c>
+      <c r="A66" s="19"/>
+      <c r="B66" s="17"/>
       <c r="C66" s="17"/>
-      <c r="D66" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>7</v>
-      </c>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
       <c r="F66" s="17"/>
-      <c r="I66" s="6" t="s">
-        <v>129</v>
-      </c>
       <c r="J66" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A67" s="19" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C67" s="17"/>
       <c r="D67" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" s="17" t="s">
-        <v>7</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E67" s="17"/>
       <c r="F67" s="17"/>
       <c r="I67" s="6" t="s">
-        <v>102</v>
+        <v>312</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A68" s="19" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B68" s="36" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C68" s="17"/>
       <c r="D68" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E68" s="17" t="s">
-        <v>7</v>
-      </c>
+      <c r="E68" s="17"/>
       <c r="F68" s="17"/>
-      <c r="I68" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="K68" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A69" s="19" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C69" s="17"/>
       <c r="D69" s="17" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F69" s="17"/>
       <c r="I69" s="6" t="s">
-        <v>134</v>
+        <v>316</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A70" s="19" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="17" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="E70" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F70" s="17"/>
       <c r="I70" s="6" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A71" s="19" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C71" s="17"/>
       <c r="D71" s="17" t="s">
@@ -3538,21 +3470,21 @@
       </c>
       <c r="F71" s="17"/>
       <c r="I71" s="6" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A72" s="19" t="s">
-        <v>362</v>
-      </c>
-      <c r="B72" s="34" t="s">
-        <v>137</v>
+        <v>356</v>
+      </c>
+      <c r="B72" s="36" t="s">
+        <v>130</v>
       </c>
       <c r="C72" s="17"/>
       <c r="D72" s="17" t="s">
@@ -3562,177 +3494,187 @@
         <v>7</v>
       </c>
       <c r="F72" s="17"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9" t="s">
+      <c r="I72" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A73" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="17"/>
+      <c r="I73" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A74" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="B74" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="17"/>
+      <c r="I74" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A75" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="B75" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="17"/>
+      <c r="I75" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A76" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B76" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="17"/>
+      <c r="I76" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A77" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="B77" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="17"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="J72" s="9" t="s">
+      <c r="J77" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="K72" s="9"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A73" s="18" t="s">
+      <c r="K77" s="9"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A78" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="B73" s="37" t="s">
+      <c r="B78" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18" t="s">
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F73" s="18"/>
-      <c r="H73" s="1" t="s">
+      <c r="F78" s="18"/>
+      <c r="H78" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I73" s="6"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A74" s="18"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="41" t="s">
+      <c r="I78" s="6"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A79" s="18"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="41" t="s">
+        <v>362</v>
+      </c>
+      <c r="D79" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" s="42"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="43"/>
+      <c r="H79"/>
+      <c r="I79" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="J79" t="s">
         <v>363</v>
       </c>
-      <c r="D74" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E74" s="42"/>
-      <c r="F74" s="42"/>
-      <c r="G74" s="43"/>
-      <c r="H74"/>
-      <c r="I74" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="J74" t="s">
+      <c r="K79" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A80" s="18"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="41" t="s">
         <v>364</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A75" s="18"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="41" t="s">
-        <v>365</v>
-      </c>
-      <c r="D75" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E75" s="42"/>
-      <c r="F75" s="42"/>
-      <c r="G75" s="43"/>
-      <c r="H75"/>
-      <c r="I75" s="43" t="s">
-        <v>372</v>
-      </c>
-      <c r="J75" t="s">
-        <v>366</v>
-      </c>
-      <c r="K75" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A76" s="18"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="41" t="s">
-        <v>367</v>
-      </c>
-      <c r="D76" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E76" s="42"/>
-      <c r="F76" s="42"/>
-      <c r="G76" s="43"/>
-      <c r="H76"/>
-      <c r="I76" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="J76" t="s">
-        <v>366</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A77" s="18"/>
-      <c r="B77" s="37"/>
-      <c r="C77" s="41" t="s">
-        <v>368</v>
-      </c>
-      <c r="D77" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="E77" s="42"/>
-      <c r="F77" s="42"/>
-      <c r="G77" s="43"/>
-      <c r="H77"/>
-      <c r="I77" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="J77" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A78" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B78" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" s="4"/>
-      <c r="H78" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I78" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="J78" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="K78" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A79" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B79" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" s="4"/>
-      <c r="H79" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I79" s="6"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A80" s="4"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="41" t="s">
-        <v>363</v>
       </c>
       <c r="D80" s="41" t="s">
         <v>5</v>
@@ -3741,21 +3683,21 @@
       <c r="F80" s="42"/>
       <c r="G80" s="43"/>
       <c r="H80"/>
-      <c r="I80" s="44" t="s">
+      <c r="I80" s="43" t="s">
         <v>371</v>
       </c>
       <c r="J80" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A81" s="4"/>
-      <c r="B81" s="24"/>
+      <c r="A81" s="18"/>
+      <c r="B81" s="37"/>
       <c r="C81" s="41" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D81" s="41" t="s">
         <v>5</v>
@@ -3768,482 +3710,501 @@
         <v>372</v>
       </c>
       <c r="J81" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A82" s="4"/>
-      <c r="B82" s="24"/>
+      <c r="A82" s="18"/>
+      <c r="B82" s="37"/>
       <c r="C82" s="41" t="s">
         <v>367</v>
       </c>
       <c r="D82" s="41" t="s">
-        <v>5</v>
+        <v>368</v>
       </c>
       <c r="E82" s="42"/>
       <c r="F82" s="42"/>
       <c r="G82" s="43"/>
       <c r="H82"/>
-      <c r="I82" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="J82" t="s">
-        <v>366</v>
+      <c r="I82" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>382</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A83" s="4"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="41" t="s">
-        <v>368</v>
-      </c>
-      <c r="D83" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="E83" s="42"/>
-      <c r="F83" s="42"/>
-      <c r="G83" s="43"/>
-      <c r="H83"/>
+      <c r="A83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B83" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="4"/>
+      <c r="H83" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="I83" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>182</v>
+        <v>299</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>240</v>
+        <v>329</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A84" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B84" s="22" t="s">
-        <v>370</v>
+        <v>53</v>
+      </c>
+      <c r="B84" s="24" t="s">
+        <v>14</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F84" s="4"/>
       <c r="H84" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="I84" s="6"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A85" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B85" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="4"/>
-      <c r="I85" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="J85" s="1" t="s">
-        <v>184</v>
+      <c r="A85" s="4"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="41" t="s">
+        <v>362</v>
+      </c>
+      <c r="D85" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85" s="42"/>
+      <c r="F85" s="42"/>
+      <c r="G85" s="43"/>
+      <c r="H85"/>
+      <c r="I85" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="J85" t="s">
+        <v>363</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>221</v>
+        <v>379</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A86" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B86" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F86" s="4"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="41" t="s">
+        <v>364</v>
+      </c>
+      <c r="D86" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="42"/>
+      <c r="F86" s="42"/>
+      <c r="G86" s="43"/>
+      <c r="H86"/>
+      <c r="I86" s="43" t="s">
+        <v>371</v>
+      </c>
+      <c r="J86" t="s">
+        <v>365</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A87" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B87" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F87" s="4"/>
-      <c r="H87" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="I87" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>184</v>
+      <c r="A87" s="4"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="41" t="s">
+        <v>366</v>
+      </c>
+      <c r="D87" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" s="42"/>
+      <c r="F87" s="42"/>
+      <c r="G87" s="43"/>
+      <c r="H87"/>
+      <c r="I87" s="43" t="s">
+        <v>372</v>
+      </c>
+      <c r="J87" t="s">
+        <v>365</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>242</v>
+        <v>381</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="H88" s="7"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="41" t="s">
+        <v>367</v>
+      </c>
+      <c r="D88" s="41" t="s">
+        <v>368</v>
+      </c>
+      <c r="E88" s="42"/>
+      <c r="F88" s="42"/>
+      <c r="G88" s="43"/>
+      <c r="H88"/>
       <c r="I88" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="J88" s="13" t="s">
-        <v>184</v>
+        <v>323</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A89" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B89" s="24" t="s">
-        <v>14</v>
+        <v>54</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>369</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F89" s="4"/>
       <c r="H89" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I89" s="6"/>
+        <v>189</v>
+      </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A90" s="4"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="41" t="s">
-        <v>363</v>
-      </c>
-      <c r="D90" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E90" s="42"/>
-      <c r="F90" s="42"/>
-      <c r="G90" s="43"/>
-      <c r="H90"/>
-      <c r="I90" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="J90" t="s">
-        <v>364</v>
+      <c r="A90" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B90" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="4"/>
+      <c r="I90" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>383</v>
+        <v>221</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A91" s="4"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="41" t="s">
-        <v>365</v>
-      </c>
-      <c r="D91" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E91" s="42"/>
-      <c r="F91" s="42"/>
-      <c r="G91" s="43"/>
-      <c r="H91"/>
-      <c r="I91" s="43" t="s">
-        <v>372</v>
-      </c>
-      <c r="J91" t="s">
-        <v>366</v>
-      </c>
-      <c r="K91" s="1" t="s">
-        <v>384</v>
-      </c>
+      <c r="A91" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="4"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A92" s="4"/>
-      <c r="B92" s="24"/>
-      <c r="C92" s="41" t="s">
-        <v>367</v>
-      </c>
-      <c r="D92" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E92" s="42"/>
-      <c r="F92" s="42"/>
-      <c r="G92" s="43"/>
-      <c r="H92"/>
-      <c r="I92" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="J92" t="s">
-        <v>366</v>
+      <c r="A92" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B92" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92" s="4"/>
+      <c r="H92" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="I92" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>385</v>
+        <v>242</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A93" s="4"/>
-      <c r="B93" s="24"/>
-      <c r="C93" s="41" t="s">
-        <v>368</v>
-      </c>
-      <c r="D93" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="E93" s="42"/>
-      <c r="F93" s="42"/>
-      <c r="G93" s="43"/>
-      <c r="H93"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="H93" s="7"/>
       <c r="I93" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>182</v>
+        <v>321</v>
+      </c>
+      <c r="J93" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>386</v>
+        <v>241</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A94" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="4"/>
+      <c r="H94" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I94" s="6"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A95" s="4"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="41" t="s">
+        <v>362</v>
+      </c>
+      <c r="D95" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E95" s="42"/>
+      <c r="F95" s="42"/>
+      <c r="G95" s="43"/>
+      <c r="H95"/>
+      <c r="I95" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="J95" t="s">
+        <v>363</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A96" s="4"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="41" t="s">
+        <v>364</v>
+      </c>
+      <c r="D96" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" s="42"/>
+      <c r="F96" s="42"/>
+      <c r="G96" s="43"/>
+      <c r="H96"/>
+      <c r="I96" s="43" t="s">
+        <v>371</v>
+      </c>
+      <c r="J96" t="s">
+        <v>365</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A97" s="4"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="41" t="s">
+        <v>366</v>
+      </c>
+      <c r="D97" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="43"/>
+      <c r="H97"/>
+      <c r="I97" s="43" t="s">
+        <v>372</v>
+      </c>
+      <c r="J97" t="s">
+        <v>365</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A98" s="4"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="41" t="s">
+        <v>367</v>
+      </c>
+      <c r="D98" s="41" t="s">
+        <v>368</v>
+      </c>
+      <c r="E98" s="42"/>
+      <c r="F98" s="42"/>
+      <c r="G98" s="43"/>
+      <c r="H98"/>
+      <c r="I98" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A99" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B94" s="23" t="s">
+      <c r="B99" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F94" s="4"/>
-      <c r="H94" s="7" t="s">
+      <c r="C99" s="4"/>
+      <c r="D99" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" s="4"/>
+      <c r="H99" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="I94" s="6" t="s">
+      <c r="I99" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="J94" s="5" t="s">
+      <c r="J99" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="K94" s="1" t="s">
+      <c r="K99" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A95" s="14"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="14"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="H95" s="7"/>
-      <c r="I95" s="6" t="s">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A100" s="14"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="J95" s="5" t="s">
+      <c r="J100" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="K95" s="1" t="s">
+      <c r="K100" s="1" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A96" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B96" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C96" s="16"/>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
-      <c r="K96" s="8"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A97" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="B97" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C97" s="16"/>
-      <c r="D97" s="16"/>
-      <c r="E97" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F97" s="16"/>
-      <c r="G97" s="9"/>
-      <c r="H97" s="9"/>
-      <c r="I97" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J97" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="K97" s="9"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A98" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="B98" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C98" s="16"/>
-      <c r="D98" s="16"/>
-      <c r="E98" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F98" s="16"/>
-      <c r="K98" s="8"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A99" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C99" s="16"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="K99" s="8"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A100" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="B100" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C100" s="16"/>
-      <c r="D100" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E100" s="16"/>
-      <c r="F100" s="16"/>
-      <c r="I100" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="J100" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K100" s="8" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A101" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="B101" s="31" t="s">
-        <v>81</v>
+        <v>176</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>75</v>
       </c>
       <c r="C101" s="16"/>
-      <c r="D101" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E101" s="16" t="s">
-        <v>9</v>
-      </c>
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
       <c r="F101" s="16"/>
-      <c r="K101" s="8" t="s">
-        <v>284</v>
-      </c>
+      <c r="K101" s="8"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A102" s="15"/>
-      <c r="B102" s="16"/>
-      <c r="C102" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>5</v>
-      </c>
+      <c r="A102" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B102" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C102" s="16"/>
+      <c r="D102" s="16"/>
       <c r="E102" s="16" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="F102" s="16"/>
-      <c r="K102" s="8" t="s">
-        <v>285</v>
-      </c>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J102" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K102" s="9"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A103" s="15"/>
-      <c r="B103" s="16"/>
+      <c r="A103" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" s="29" t="s">
+        <v>78</v>
+      </c>
       <c r="C103" s="16"/>
       <c r="D103" s="16"/>
-      <c r="E103" s="16"/>
+      <c r="E103" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="F103" s="16"/>
-      <c r="J103" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K103" s="8" t="s">
-        <v>286</v>
-      </c>
+      <c r="K103" s="8"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A104" s="15" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="B104" s="30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C104" s="16"/>
-      <c r="D104" s="16" t="s">
-        <v>86</v>
-      </c>
+      <c r="D104" s="16"/>
       <c r="E104" s="16"/>
       <c r="F104" s="16"/>
-      <c r="I104" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="J104" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K104" s="8" t="s">
-        <v>290</v>
-      </c>
+      <c r="K104" s="8"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A105" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B105" s="30" t="s">
-        <v>88</v>
+        <v>180</v>
+      </c>
+      <c r="B105" s="31" t="s">
+        <v>80</v>
       </c>
       <c r="C105" s="16"/>
       <c r="D105" s="16" t="s">
@@ -4251,189 +4212,160 @@
       </c>
       <c r="E105" s="16"/>
       <c r="F105" s="16"/>
+      <c r="I105" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="K105" s="8" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A106" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B106" s="30" t="s">
-        <v>89</v>
+        <v>158</v>
+      </c>
+      <c r="B106" s="31" t="s">
+        <v>81</v>
       </c>
       <c r="C106" s="16"/>
       <c r="D106" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E106" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="E106" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="F106" s="16"/>
-      <c r="I106" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="J106" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="K106" s="8" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A107" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B107" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C107" s="16"/>
+      <c r="A107" s="15"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="D107" s="16" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="E107" s="16" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="F107" s="16"/>
-      <c r="I107" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="J107" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="K107" s="8" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A108" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="B108" s="30" t="s">
-        <v>93</v>
-      </c>
+      <c r="A108" s="15"/>
+      <c r="B108" s="16"/>
       <c r="C108" s="16"/>
-      <c r="D108" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E108" s="16" t="s">
-        <v>7</v>
-      </c>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
       <c r="F108" s="16"/>
-      <c r="I108" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="J108" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K108" s="8" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A109" s="15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C109" s="16"/>
       <c r="D109" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E109" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E109" s="16"/>
       <c r="F109" s="16"/>
       <c r="I109" s="6" t="s">
-        <v>97</v>
+        <v>313</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>212</v>
+        <v>87</v>
       </c>
       <c r="K109" s="8" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A110" s="15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C110" s="16"/>
       <c r="D110" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E110" s="16"/>
       <c r="F110" s="16"/>
-      <c r="I110" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="J110" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="K110" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A111" s="15" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B111" s="30" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C111" s="16"/>
       <c r="D111" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E111" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E111" s="16"/>
       <c r="F111" s="16"/>
       <c r="I111" s="6" t="s">
-        <v>102</v>
+        <v>320</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K111" s="8" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A112" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="B112" s="31" t="s">
-        <v>103</v>
+        <v>162</v>
+      </c>
+      <c r="B112" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="C112" s="16"/>
       <c r="D112" s="16" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="E112" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F112" s="16"/>
       <c r="I112" s="6" t="s">
-        <v>104</v>
+        <v>317</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="K112" s="8" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A113" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B113" s="31" t="s">
-        <v>105</v>
+        <v>163</v>
+      </c>
+      <c r="B113" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="C113" s="16"/>
       <c r="D113" s="16" t="s">
@@ -4444,46 +4376,46 @@
       </c>
       <c r="F113" s="16"/>
       <c r="I113" s="6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="K113" s="8" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A114" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B114" s="31" t="s">
-        <v>108</v>
+        <v>164</v>
+      </c>
+      <c r="B114" s="30" t="s">
+        <v>96</v>
       </c>
       <c r="C114" s="16"/>
       <c r="D114" s="16" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="E114" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F114" s="16"/>
       <c r="I114" s="6" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>100</v>
+        <v>212</v>
       </c>
       <c r="K114" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A115" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B115" s="31" t="s">
-        <v>110</v>
+        <v>165</v>
+      </c>
+      <c r="B115" s="30" t="s">
+        <v>98</v>
       </c>
       <c r="C115" s="16"/>
       <c r="D115" s="16" t="s">
@@ -4493,22 +4425,22 @@
         <v>7</v>
       </c>
       <c r="F115" s="16"/>
-      <c r="G115" s="9"/>
-      <c r="H115" s="9"/>
-      <c r="I115" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="J115" s="9" t="s">
+      <c r="I115" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J115" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K115" s="9"/>
+      <c r="K115" s="8" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A116" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B116" s="31" t="s">
-        <v>112</v>
+        <v>166</v>
+      </c>
+      <c r="B116" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C116" s="16"/>
       <c r="D116" s="16" t="s">
@@ -4519,21 +4451,21 @@
       </c>
       <c r="F116" s="16"/>
       <c r="I116" s="6" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="J116" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K116" s="8" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A117" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B117" s="29" t="s">
-        <v>114</v>
+        <v>167</v>
+      </c>
+      <c r="B117" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="C117" s="16"/>
       <c r="D117" s="16" t="s">
@@ -4543,154 +4475,185 @@
         <v>7</v>
       </c>
       <c r="F117" s="16"/>
-      <c r="G117" s="10"/>
-      <c r="H117" s="10"/>
-      <c r="I117" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="J117" s="11" t="s">
+      <c r="I117" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J117" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K117" s="9"/>
+      <c r="K117" s="8" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A118" s="19" t="s">
-        <v>334</v>
-      </c>
-      <c r="B118" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="C118" s="17"/>
-      <c r="D118" s="17"/>
-      <c r="E118" s="17"/>
-      <c r="F118" s="17"/>
+      <c r="A118" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B118" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C118" s="16"/>
+      <c r="D118" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E118" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118" s="16"/>
+      <c r="I118" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K118" s="8" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A119" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="B119" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C119" s="17"/>
-      <c r="D119" s="17"/>
-      <c r="E119" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F119" s="17"/>
+      <c r="A119" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B119" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C119" s="16"/>
+      <c r="D119" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E119" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F119" s="16"/>
+      <c r="I119" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K119" s="8" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A120" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B120" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="C120" s="17"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="17"/>
+      <c r="A120" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B120" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C120" s="16"/>
+      <c r="D120" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F120" s="16"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J120" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K120" s="9"/>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A121" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="B121" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="C121" s="17"/>
-      <c r="D121" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E121" s="17"/>
-      <c r="F121" s="17"/>
+      <c r="A121" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B121" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C121" s="16"/>
+      <c r="D121" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E121" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F121" s="16"/>
       <c r="I121" s="6" t="s">
-        <v>309</v>
+        <v>113</v>
       </c>
       <c r="J121" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K121" s="1" t="s">
-        <v>248</v>
+      <c r="K121" s="8" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A122" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="B122" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="C122" s="17"/>
-      <c r="D122" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E122" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F122" s="17"/>
-      <c r="K122" s="1" t="s">
-        <v>249</v>
-      </c>
+      <c r="A122" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B122" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C122" s="16"/>
+      <c r="D122" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F122" s="16"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J122" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K122" s="9"/>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A123" s="19"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D123" s="17" t="s">
-        <v>5</v>
-      </c>
+      <c r="A123" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="B123" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C123" s="17"/>
+      <c r="D123" s="17"/>
       <c r="E123" s="17"/>
       <c r="F123" s="17"/>
-      <c r="K123" s="1" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A124" s="19"/>
-      <c r="B124" s="17"/>
+      <c r="A124" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B124" s="32" t="s">
+        <v>117</v>
+      </c>
       <c r="C124" s="17"/>
       <c r="D124" s="17"/>
-      <c r="E124" s="17"/>
+      <c r="E124" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="F124" s="17"/>
-      <c r="J124" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K124" s="1" t="s">
-        <v>251</v>
-      </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A125" s="19" t="s">
-        <v>336</v>
+        <v>174</v>
       </c>
       <c r="B125" s="33" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C125" s="17"/>
-      <c r="D125" s="17" t="s">
-        <v>86</v>
-      </c>
+      <c r="D125" s="17"/>
       <c r="E125" s="17"/>
       <c r="F125" s="17"/>
-      <c r="I125" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="J125" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K125" s="1" t="s">
-        <v>254</v>
-      </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A126" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="B126" s="33" t="s">
-        <v>123</v>
+        <v>175</v>
+      </c>
+      <c r="B126" s="34" t="s">
+        <v>119</v>
       </c>
       <c r="C126" s="17"/>
       <c r="D126" s="17" t="s">
@@ -4698,191 +4661,160 @@
       </c>
       <c r="E126" s="17"/>
       <c r="F126" s="17"/>
+      <c r="I126" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="K126" s="1" t="s">
-        <v>331</v>
+        <v>248</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A127" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="B127" s="33" t="s">
-        <v>124</v>
+        <v>334</v>
+      </c>
+      <c r="B127" s="34" t="s">
+        <v>120</v>
       </c>
       <c r="C127" s="17"/>
       <c r="D127" s="17" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="E127" s="17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F127" s="17"/>
-      <c r="I127" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="J127" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="K127" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A128" s="19" t="s">
-        <v>339</v>
-      </c>
-      <c r="B128" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C128" s="17"/>
+      <c r="A128" s="19"/>
+      <c r="B128" s="17"/>
+      <c r="C128" s="17" t="s">
+        <v>121</v>
+      </c>
       <c r="D128" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="E128" s="17" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E128" s="17"/>
       <c r="F128" s="17"/>
-      <c r="I128" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J128" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="K128" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A129" s="19" t="s">
-        <v>340</v>
-      </c>
-      <c r="B129" s="33" t="s">
-        <v>128</v>
-      </c>
+      <c r="A129" s="19"/>
+      <c r="B129" s="17"/>
       <c r="C129" s="17"/>
-      <c r="D129" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E129" s="17" t="s">
-        <v>7</v>
-      </c>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
       <c r="F129" s="17"/>
-      <c r="I129" s="6" t="s">
-        <v>129</v>
-      </c>
       <c r="J129" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A130" s="19" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B130" s="33" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C130" s="17"/>
       <c r="D130" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E130" s="17" t="s">
-        <v>7</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E130" s="17"/>
       <c r="F130" s="17"/>
       <c r="I130" s="6" t="s">
-        <v>102</v>
+        <v>314</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A131" s="19" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B131" s="33" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C131" s="17"/>
       <c r="D131" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E131" s="17" t="s">
-        <v>7</v>
-      </c>
+      <c r="E131" s="17"/>
       <c r="F131" s="17"/>
-      <c r="I131" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="J131" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="K131" s="1" t="s">
-        <v>259</v>
+        <v>330</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A132" s="19" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B132" s="33" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C132" s="17"/>
       <c r="D132" s="17" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="E132" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F132" s="17"/>
       <c r="I132" s="6" t="s">
-        <v>134</v>
+        <v>318</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A133" s="19" t="s">
-        <v>344</v>
-      </c>
-      <c r="B133" s="34" t="s">
-        <v>135</v>
+        <v>338</v>
+      </c>
+      <c r="B133" s="33" t="s">
+        <v>126</v>
       </c>
       <c r="C133" s="17"/>
       <c r="D133" s="17" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="E133" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F133" s="17"/>
       <c r="I133" s="6" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A134" s="19" t="s">
-        <v>345</v>
-      </c>
-      <c r="B134" s="34" t="s">
-        <v>136</v>
+        <v>339</v>
+      </c>
+      <c r="B134" s="33" t="s">
+        <v>128</v>
       </c>
       <c r="C134" s="17"/>
       <c r="D134" s="17" t="s">
@@ -4893,221 +4825,235 @@
       </c>
       <c r="F134" s="17"/>
       <c r="I134" s="6" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>73</v>
       </c>
       <c r="K134" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A135" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="B135" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C135" s="17"/>
+      <c r="D135" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E135" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F135" s="17"/>
+      <c r="I135" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A136" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="B136" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C136" s="17"/>
+      <c r="D136" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E136" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F136" s="17"/>
+      <c r="I136" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A137" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B137" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C137" s="17"/>
+      <c r="D137" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E137" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F137" s="17"/>
+      <c r="I137" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A138" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="B138" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E138" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F138" s="17"/>
+      <c r="I138" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A139" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="B139" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="C139" s="17"/>
+      <c r="D139" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E139" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F139" s="17"/>
+      <c r="I139" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K139" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A135" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="B135" s="39" t="s">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A140" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="B140" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="C135" s="9"/>
-      <c r="D135" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F135" s="9"/>
-      <c r="G135" s="9"/>
-      <c r="H135" s="9"/>
-      <c r="I135" s="9" t="s">
+      <c r="C140" s="9"/>
+      <c r="D140" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E140" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="J135" s="9" t="s">
+      <c r="J140" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="K135" s="9"/>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A136" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B136" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C136" s="4"/>
-      <c r="D136" s="4"/>
-      <c r="E136" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F136" s="4"/>
-      <c r="H136" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I136" s="6"/>
-      <c r="J136" s="5"/>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A137" s="4"/>
-      <c r="B137" s="24"/>
-      <c r="C137" s="41" t="s">
-        <v>363</v>
-      </c>
-      <c r="D137" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E137" s="42"/>
-      <c r="F137" s="42"/>
-      <c r="G137" s="43"/>
-      <c r="H137"/>
-      <c r="I137" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="J137" t="s">
-        <v>364</v>
-      </c>
-      <c r="K137" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A138" s="4"/>
-      <c r="B138" s="24"/>
-      <c r="C138" s="41" t="s">
-        <v>365</v>
-      </c>
-      <c r="D138" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E138" s="42"/>
-      <c r="F138" s="42"/>
-      <c r="G138" s="43"/>
-      <c r="H138"/>
-      <c r="I138" s="43" t="s">
-        <v>372</v>
-      </c>
-      <c r="J138" t="s">
-        <v>366</v>
-      </c>
-      <c r="K138" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A139" s="4"/>
-      <c r="B139" s="24"/>
-      <c r="C139" s="41" t="s">
-        <v>367</v>
-      </c>
-      <c r="D139" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E139" s="42"/>
-      <c r="F139" s="42"/>
-      <c r="G139" s="43"/>
-      <c r="H139"/>
-      <c r="I139" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="J139" t="s">
-        <v>366</v>
-      </c>
-      <c r="K139" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A140" s="4"/>
-      <c r="B140" s="24"/>
-      <c r="C140" s="41" t="s">
-        <v>368</v>
-      </c>
-      <c r="D140" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="E140" s="42"/>
-      <c r="F140" s="42"/>
-      <c r="G140" s="43"/>
-      <c r="H140"/>
-      <c r="I140" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="J140" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K140" s="1" t="s">
-        <v>245</v>
-      </c>
+      <c r="K140" s="9"/>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A141" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B141" s="23" t="s">
-        <v>65</v>
+        <v>211</v>
+      </c>
+      <c r="B141" s="24" t="s">
+        <v>14</v>
       </c>
       <c r="C141" s="4"/>
-      <c r="D141" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D141" s="4"/>
       <c r="E141" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F141" s="4"/>
-      <c r="H141" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="I141" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="J141" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="K141" s="1" t="s">
-        <v>247</v>
-      </c>
+      <c r="H141" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I141" s="6"/>
+      <c r="J141" s="5"/>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A142" s="4"/>
-      <c r="B142" s="4"/>
-      <c r="C142" s="4"/>
-      <c r="D142" s="4"/>
-      <c r="E142" s="4"/>
-      <c r="F142" s="4"/>
-      <c r="H142" s="7"/>
-      <c r="I142" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="J142" s="5" t="s">
-        <v>184</v>
+      <c r="B142" s="24"/>
+      <c r="C142" s="41" t="s">
+        <v>362</v>
+      </c>
+      <c r="D142" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E142" s="42"/>
+      <c r="F142" s="42"/>
+      <c r="G142" s="43"/>
+      <c r="H142"/>
+      <c r="I142" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="J142" t="s">
+        <v>363</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>246</v>
+        <v>386</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A143" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B143" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
-      <c r="E143" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F143" s="4"/>
-      <c r="H143" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I143" s="6"/>
-      <c r="J143" s="5"/>
+      <c r="A143" s="4"/>
+      <c r="B143" s="24"/>
+      <c r="C143" s="41" t="s">
+        <v>364</v>
+      </c>
+      <c r="D143" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E143" s="42"/>
+      <c r="F143" s="42"/>
+      <c r="G143" s="43"/>
+      <c r="H143"/>
+      <c r="I143" s="43" t="s">
+        <v>371</v>
+      </c>
+      <c r="J143" t="s">
+        <v>365</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A144" s="4"/>
       <c r="B144" s="24"/>
       <c r="C144" s="41" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D144" s="41" t="s">
         <v>5</v>
@@ -5116,137 +5062,248 @@
       <c r="F144" s="42"/>
       <c r="G144" s="43"/>
       <c r="H144"/>
-      <c r="I144" s="44" t="s">
-        <v>371</v>
+      <c r="I144" s="43" t="s">
+        <v>372</v>
       </c>
       <c r="J144" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A145" s="4"/>
       <c r="B145" s="24"/>
       <c r="C145" s="41" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D145" s="41" t="s">
-        <v>5</v>
+        <v>368</v>
       </c>
       <c r="E145" s="42"/>
       <c r="F145" s="42"/>
       <c r="G145" s="43"/>
       <c r="H145"/>
-      <c r="I145" s="43" t="s">
-        <v>372</v>
-      </c>
-      <c r="J145" t="s">
-        <v>366</v>
+      <c r="I145" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>391</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A146" s="4"/>
-      <c r="B146" s="24"/>
-      <c r="C146" s="41" t="s">
-        <v>367</v>
-      </c>
-      <c r="D146" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E146" s="42"/>
-      <c r="F146" s="42"/>
-      <c r="G146" s="43"/>
-      <c r="H146"/>
-      <c r="I146" s="43" t="s">
-        <v>373</v>
-      </c>
-      <c r="J146" t="s">
-        <v>366</v>
+      <c r="A146" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B146" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E146" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F146" s="4"/>
+      <c r="H146" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="I146" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="J146" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>392</v>
+        <v>247</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A147" s="4"/>
-      <c r="B147" s="24"/>
-      <c r="C147" s="41" t="s">
-        <v>368</v>
-      </c>
-      <c r="D147" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="E147" s="42"/>
-      <c r="F147" s="42"/>
-      <c r="G147" s="43"/>
-      <c r="H147"/>
+      <c r="B147" s="4"/>
+      <c r="C147" s="4"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="H147" s="7"/>
       <c r="I147" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="J147" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
+      </c>
+      <c r="J147" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>393</v>
+        <v>246</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A148" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B148" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="B148" s="24" t="s">
+        <v>14</v>
       </c>
       <c r="C148" s="4"/>
-      <c r="D148" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F148" s="4"/>
       <c r="H148" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="I148" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="I148" s="6"/>
+      <c r="J148" s="5"/>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A149" s="4"/>
+      <c r="B149" s="24"/>
+      <c r="C149" s="41" t="s">
+        <v>362</v>
+      </c>
+      <c r="D149" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E149" s="42"/>
+      <c r="F149" s="42"/>
+      <c r="G149" s="43"/>
+      <c r="H149"/>
+      <c r="I149" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="J149" t="s">
+        <v>363</v>
+      </c>
+      <c r="K149" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A150" s="4"/>
+      <c r="B150" s="24"/>
+      <c r="C150" s="41" t="s">
+        <v>364</v>
+      </c>
+      <c r="D150" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E150" s="42"/>
+      <c r="F150" s="42"/>
+      <c r="G150" s="43"/>
+      <c r="H150"/>
+      <c r="I150" s="43" t="s">
+        <v>371</v>
+      </c>
+      <c r="J150" t="s">
+        <v>365</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A151" s="4"/>
+      <c r="B151" s="24"/>
+      <c r="C151" s="41" t="s">
+        <v>366</v>
+      </c>
+      <c r="D151" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E151" s="42"/>
+      <c r="F151" s="42"/>
+      <c r="G151" s="43"/>
+      <c r="H151"/>
+      <c r="I151" s="43" t="s">
+        <v>372</v>
+      </c>
+      <c r="J151" t="s">
+        <v>365</v>
+      </c>
+      <c r="K151" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A152" s="4"/>
+      <c r="B152" s="24"/>
+      <c r="C152" s="41" t="s">
+        <v>367</v>
+      </c>
+      <c r="D152" s="41" t="s">
+        <v>368</v>
+      </c>
+      <c r="E152" s="42"/>
+      <c r="F152" s="42"/>
+      <c r="G152" s="43"/>
+      <c r="H152"/>
+      <c r="I152" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J152" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K152" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A153" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B153" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C153" s="4"/>
+      <c r="D153" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F153" s="4"/>
+      <c r="H153" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="J148" s="5" t="s">
+      <c r="I153" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="J153" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="K148" s="1" t="s">
+      <c r="K153" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B150" s="5"/>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B151" s="5" t="s">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B155" s="5"/>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B156" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I151" s="1" t="s">
+      <c r="I156" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="I152" s="1" t="s">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I157" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="I153" s="1" t="s">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I158" s="1" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A1:XFD26 A27:H27 L27:XFD27 A136:J136 L136:XFD136 A137:XFD142 A143:J143 L143:XFD143 A144:XFD1048576 A89:J89 L89:XFD89 A90:XFD135 A28:XFD72 A73:J73 L73:XFD73 A74:XFD78 A79:J79 L79:XFD79 A80:XFD88">
+  <conditionalFormatting sqref="A32:H32 L32:XFD32 A141:J141 L141:XFD141 A142:XFD147 A148:J148 L148:XFD148 A149:XFD1048576 A94:J94 L94:XFD94 A95:XFD140 A33:XFD77 A78:J78 L78:XFD78 A79:XFD83 A84:J84 L84:XFD84 A85:XFD93 A1:XFD24 A25:J25 L25:XFD25 A26:XFD31">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
@@ -5263,68 +5320,68 @@
     <hyperlink ref="I21" location="Sheet2!$B$353" display="Name of object"/>
     <hyperlink ref="I22" location="Sheet2!$B$363" display="Clinical description"/>
     <hyperlink ref="I23" location="Sheet2!$B$373" display="Interpretation"/>
-    <hyperlink ref="I25" location="Sheet2!$B$410" display="URI to original data1"/>
-    <hyperlink ref="I26" location="Sheet2!$B$567" display="Progress Note3"/>
-    <hyperlink ref="I31" location="Sheet2!$B$597" display="URI to original data2"/>
-    <hyperlink ref="I32" location="Sheet2!$B$639" display="Progress Note4"/>
-    <hyperlink ref="I37" location="Sheet2!$B$740" display="Medication1"/>
-    <hyperlink ref="I41" location="Sheet2!$B$805" display="Dose amount1"/>
-    <hyperlink ref="I43" location="Sheet2!$B$824" display="Frequency1"/>
-    <hyperlink ref="I44" location="Sheet2!$B$884" display="Order start date/time1"/>
-    <hyperlink ref="I45" location="Sheet2!$B$844" display="Direction duration"/>
-    <hyperlink ref="I46" location="Sheet2!$B$868" display="Patient instruction"/>
-    <hyperlink ref="I47" location="Sheet2!$B$834" display="As required"/>
-    <hyperlink ref="I48" location="Sheet2!$B$773" display="Route"/>
-    <hyperlink ref="I49" location="Sheet2!$B$763" display="Preparation form"/>
-    <hyperlink ref="I50" location="Sheet2!$B$789" display="Direction sequence"/>
-    <hyperlink ref="I51" location="Sheet2!$B$914" display="substitution permitted"/>
-    <hyperlink ref="I53" location="Sheet2!$B$858" display="Additional instruction"/>
-    <hyperlink ref="I58" location="Sheet2!$B$973" display="Medication2"/>
-    <hyperlink ref="I62" location="Sheet2!$B$1035" display="Dose amount2"/>
-    <hyperlink ref="I64" location="Sheet2!$B$1071" display="Order start date/time2"/>
-    <hyperlink ref="I65" location="Sheet2!$B$1081" display="Order stop date/time"/>
-    <hyperlink ref="I66" location="Sheet2!$B$1101" display="Administration instruction"/>
-    <hyperlink ref="I67" location="Sheet2!$B$993" display="Route"/>
-    <hyperlink ref="I68" location="Sheet2!$B$1111" display="Site"/>
-    <hyperlink ref="I69" location="Sheet2!$B$1125" display="Delivery method"/>
-    <hyperlink ref="I70" location="Sheet2!$B$1019" display="Direction sequence"/>
-    <hyperlink ref="I71" location="Sheet2!$B$1055" display="Additional instruction"/>
-    <hyperlink ref="I78" location="Sheet2!$B$711" display="Progress Note5"/>
-    <hyperlink ref="I85" location="Sheet2!$B$1238" display="Synopsis"/>
-    <hyperlink ref="I87" location="Sheet2!$B$1287" display="Description2"/>
-    <hyperlink ref="I88" location="Sheet2!$B$1277" display="*1)Service name"/>
-    <hyperlink ref="I94" location="Sheet2!$B$1371" display="Description3"/>
-    <hyperlink ref="I95" location="Sheet2!$B$1361" display="*2)Service name"/>
-    <hyperlink ref="I100" location="Sheet2!$B$1579" display="Medication3"/>
-    <hyperlink ref="I104" location="Sheet2!$B$1644" display="Dose amount3"/>
-    <hyperlink ref="I106" location="Sheet2!$B$1663" display="Frequency2"/>
-    <hyperlink ref="I107" location="Sheet2!$B$1737" display="Order start date/time3"/>
-    <hyperlink ref="I108" location="Sheet2!$B$1697" display="Direction duration"/>
-    <hyperlink ref="I109" location="Sheet2!$B$1721" display="Patient instruction"/>
-    <hyperlink ref="I110" location="Sheet2!$B$1687" display="As required"/>
-    <hyperlink ref="I111" location="Sheet2!$B$1612" display="Route"/>
-    <hyperlink ref="I112" location="Sheet2!$B$1602" display="Preparation form"/>
-    <hyperlink ref="I113" location="Sheet2!$B$1628" display="Direction sequence"/>
-    <hyperlink ref="I114" location="Sheet2!$B$1767" display="substitution permitted"/>
-    <hyperlink ref="I116" location="Sheet2!$B$1711" display="Additional instruction"/>
-    <hyperlink ref="I121" location="Sheet2!$B$1836" display="Medication4"/>
-    <hyperlink ref="I125" location="Sheet2!$B$1898" display="Dose amount4"/>
-    <hyperlink ref="I127" location="Sheet2!$B$1934" display="Order start date/time4"/>
-    <hyperlink ref="I128" location="Sheet2!$B$1944" display="Order stop date/time"/>
-    <hyperlink ref="I129" location="Sheet2!$B$1964" display="Administration instruction"/>
-    <hyperlink ref="I130" location="Sheet2!$B$1856" display="Route"/>
-    <hyperlink ref="I131" location="Sheet2!$B$1974" display="Site"/>
-    <hyperlink ref="I132" location="Sheet2!$B$1988" display="Delivery method"/>
-    <hyperlink ref="I133" location="Sheet2!$B$1882" display="Direction sequence"/>
-    <hyperlink ref="I134" location="Sheet2!$B$1918" display="Additional instruction"/>
-    <hyperlink ref="I141" location="Sheet2!$B$1455" display="Description4"/>
-    <hyperlink ref="I142" location="Sheet2!$B$1445" display="*3)Service name"/>
-    <hyperlink ref="I148" location="Sheet2!$B$1535" display="Description5"/>
-    <hyperlink ref="I77" location="Sheet2!$B$597" display="URI to original data2"/>
-    <hyperlink ref="I93" location="Sheet2!$B$597" display="URI to original data2"/>
-    <hyperlink ref="I140" location="Sheet2!$B$597" display="URI to original data2"/>
-    <hyperlink ref="I147" location="Sheet2!$B$597" display="URI to original data2"/>
-    <hyperlink ref="I83" location="Sheet2!$B$597" display="URI to original data2"/>
+    <hyperlink ref="I31" location="Sheet2!$B$567" display="Progress Note3"/>
+    <hyperlink ref="I36" location="Sheet2!$B$597" display="URI to original data2"/>
+    <hyperlink ref="I37" location="Sheet2!$B$639" display="Progress Note4"/>
+    <hyperlink ref="I42" location="Sheet2!$B$740" display="Medication1"/>
+    <hyperlink ref="I46" location="Sheet2!$B$805" display="Dose amount1"/>
+    <hyperlink ref="I48" location="Sheet2!$B$824" display="Frequency1"/>
+    <hyperlink ref="I49" location="Sheet2!$B$884" display="Order start date/time1"/>
+    <hyperlink ref="I50" location="Sheet2!$B$844" display="Direction duration"/>
+    <hyperlink ref="I51" location="Sheet2!$B$868" display="Patient instruction"/>
+    <hyperlink ref="I52" location="Sheet2!$B$834" display="As required"/>
+    <hyperlink ref="I53" location="Sheet2!$B$773" display="Route"/>
+    <hyperlink ref="I54" location="Sheet2!$B$763" display="Preparation form"/>
+    <hyperlink ref="I55" location="Sheet2!$B$789" display="Direction sequence"/>
+    <hyperlink ref="I56" location="Sheet2!$B$914" display="substitution permitted"/>
+    <hyperlink ref="I58" location="Sheet2!$B$858" display="Additional instruction"/>
+    <hyperlink ref="I63" location="Sheet2!$B$973" display="Medication2"/>
+    <hyperlink ref="I67" location="Sheet2!$B$1035" display="Dose amount2"/>
+    <hyperlink ref="I69" location="Sheet2!$B$1071" display="Order start date/time2"/>
+    <hyperlink ref="I70" location="Sheet2!$B$1081" display="Order stop date/time"/>
+    <hyperlink ref="I71" location="Sheet2!$B$1101" display="Administration instruction"/>
+    <hyperlink ref="I72" location="Sheet2!$B$993" display="Route"/>
+    <hyperlink ref="I73" location="Sheet2!$B$1111" display="Site"/>
+    <hyperlink ref="I74" location="Sheet2!$B$1125" display="Delivery method"/>
+    <hyperlink ref="I75" location="Sheet2!$B$1019" display="Direction sequence"/>
+    <hyperlink ref="I76" location="Sheet2!$B$1055" display="Additional instruction"/>
+    <hyperlink ref="I83" location="Sheet2!$B$711" display="Progress Note5"/>
+    <hyperlink ref="I90" location="Sheet2!$B$1238" display="Synopsis"/>
+    <hyperlink ref="I92" location="Sheet2!$B$1287" display="Description2"/>
+    <hyperlink ref="I93" location="Sheet2!$B$1277" display="*1)Service name"/>
+    <hyperlink ref="I99" location="Sheet2!$B$1371" display="Description3"/>
+    <hyperlink ref="I100" location="Sheet2!$B$1361" display="*2)Service name"/>
+    <hyperlink ref="I105" location="Sheet2!$B$1579" display="Medication3"/>
+    <hyperlink ref="I109" location="Sheet2!$B$1644" display="Dose amount3"/>
+    <hyperlink ref="I111" location="Sheet2!$B$1663" display="Frequency2"/>
+    <hyperlink ref="I112" location="Sheet2!$B$1737" display="Order start date/time3"/>
+    <hyperlink ref="I113" location="Sheet2!$B$1697" display="Direction duration"/>
+    <hyperlink ref="I114" location="Sheet2!$B$1721" display="Patient instruction"/>
+    <hyperlink ref="I115" location="Sheet2!$B$1687" display="As required"/>
+    <hyperlink ref="I116" location="Sheet2!$B$1612" display="Route"/>
+    <hyperlink ref="I117" location="Sheet2!$B$1602" display="Preparation form"/>
+    <hyperlink ref="I118" location="Sheet2!$B$1628" display="Direction sequence"/>
+    <hyperlink ref="I119" location="Sheet2!$B$1767" display="substitution permitted"/>
+    <hyperlink ref="I121" location="Sheet2!$B$1711" display="Additional instruction"/>
+    <hyperlink ref="I126" location="Sheet2!$B$1836" display="Medication4"/>
+    <hyperlink ref="I130" location="Sheet2!$B$1898" display="Dose amount4"/>
+    <hyperlink ref="I132" location="Sheet2!$B$1934" display="Order start date/time4"/>
+    <hyperlink ref="I133" location="Sheet2!$B$1944" display="Order stop date/time"/>
+    <hyperlink ref="I134" location="Sheet2!$B$1964" display="Administration instruction"/>
+    <hyperlink ref="I135" location="Sheet2!$B$1856" display="Route"/>
+    <hyperlink ref="I136" location="Sheet2!$B$1974" display="Site"/>
+    <hyperlink ref="I137" location="Sheet2!$B$1988" display="Delivery method"/>
+    <hyperlink ref="I138" location="Sheet2!$B$1882" display="Direction sequence"/>
+    <hyperlink ref="I139" location="Sheet2!$B$1918" display="Additional instruction"/>
+    <hyperlink ref="I146" location="Sheet2!$B$1455" display="Description4"/>
+    <hyperlink ref="I147" location="Sheet2!$B$1445" display="*3)Service name"/>
+    <hyperlink ref="I153" location="Sheet2!$B$1535" display="Description5"/>
+    <hyperlink ref="I82" location="Sheet2!$B$597" display="URI to original data2"/>
+    <hyperlink ref="I98" location="Sheet2!$B$597" display="URI to original data2"/>
+    <hyperlink ref="I145" location="Sheet2!$B$597" display="URI to original data2"/>
+    <hyperlink ref="I152" location="Sheet2!$B$597" display="URI to original data2"/>
+    <hyperlink ref="I88" location="Sheet2!$B$597" display="URI to original data2"/>
+    <hyperlink ref="I29" location="Sheet2!$B$597" display="URI to original data2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>